<commit_message>
Register Test Data file Updated
</commit_message>
<xml_diff>
--- a/TestData/Register Test Data.xlsx
+++ b/TestData/Register Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAREER\Pytest Practice\CredKart 2025-26\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C8BEBE-34CB-45A3-9C01-B0F83C6284C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC07B239-A71A-4307-8E38-83BFDC10BA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +148,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,9 +189,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,7 +478,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,19 +746,19 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Screenshot function added to test_register file
</commit_message>
<xml_diff>
--- a/TestData/Register Test Data.xlsx
+++ b/TestData/Register Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAREER\Pytest Practice\CredKart 2025-26\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC07B239-A71A-4307-8E38-83BFDC10BA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9CB8AF-DCB5-4AEC-A0F4-8BE399E853F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
   <si>
     <t>RegisterName</t>
   </si>
@@ -87,9 +87,6 @@
     <t>lotus</t>
   </si>
   <si>
-    <t>lotus20@gmail.com</t>
-  </si>
-  <si>
     <t>lotus@123</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Rose</t>
   </si>
   <si>
-    <t>ROSE20@GMAIL.COM</t>
-  </si>
-  <si>
     <t>Rose@123</t>
   </si>
   <si>
@@ -117,19 +111,28 @@
     <t>cat@123</t>
   </si>
   <si>
-    <t>Pooja@22gmail.com</t>
-  </si>
-  <si>
-    <t>Pooja@23gmail.com</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
-    <t>Pooja@25gmail.com</t>
-  </si>
-  <si>
     <t>^&amp;^%$^^</t>
+  </si>
+  <si>
+    <t>Pooja@31gmail.com</t>
+  </si>
+  <si>
+    <t>lotus30@gmail.com</t>
+  </si>
+  <si>
+    <t>ROSE30@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>Pooja@35gmail.com</t>
+  </si>
+  <si>
+    <t>Pooja@32gmail.com</t>
+  </si>
+  <si>
+    <t>Pooja@33gmail.com</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -529,7 +532,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -546,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -611,7 +614,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -631,7 +634,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -654,7 +657,7 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -668,7 +671,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
@@ -682,13 +685,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -696,16 +699,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -713,16 +716,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -730,16 +733,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -747,7 +750,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>33</v>
@@ -792,21 +795,22 @@
     <hyperlink ref="B12" r:id="rId26" xr:uid="{7998B7C4-5EC9-44D5-BF82-066C2C12D792}"/>
     <hyperlink ref="C12" r:id="rId27" xr:uid="{BC535213-4FBA-45CA-9F6D-AE99CE851F26}"/>
     <hyperlink ref="D12" r:id="rId28" xr:uid="{D6303310-9468-4BA5-917A-5D96AE4DD31D}"/>
-    <hyperlink ref="B13" r:id="rId29" xr:uid="{6DBAD2B2-5A78-4383-B126-11BFA2EB73F7}"/>
-    <hyperlink ref="C13" r:id="rId30" xr:uid="{4EE4FA8F-CCC6-4931-8F70-A68DBC9220B2}"/>
-    <hyperlink ref="D13" r:id="rId31" xr:uid="{6176E101-2C7E-46F6-95A3-214967BDD8FE}"/>
-    <hyperlink ref="B14" r:id="rId32" xr:uid="{19E22425-95DB-4A99-A146-142C6BB4A91F}"/>
-    <hyperlink ref="C14" r:id="rId33" xr:uid="{1945C55F-3565-4095-BBC6-E7118079DDDE}"/>
-    <hyperlink ref="D14" r:id="rId34" xr:uid="{944F9636-C8ED-494B-97FF-2206DEA80AB1}"/>
-    <hyperlink ref="B15" r:id="rId35" xr:uid="{7CB51F97-60BB-446D-B2C6-FDDC0C3DC608}"/>
-    <hyperlink ref="C15" r:id="rId36" xr:uid="{1DB6A66C-DE77-4F09-8FE4-E1270AFC0198}"/>
-    <hyperlink ref="D15" r:id="rId37" xr:uid="{3C9CCDBA-C882-4755-B652-2B9EA3B71DDB}"/>
-    <hyperlink ref="B5" r:id="rId38" xr:uid="{68BB3A41-C871-4E8D-9E19-4F4319B95781}"/>
-    <hyperlink ref="B3" r:id="rId39" xr:uid="{8900A6CB-BC00-4A43-B105-D668EB145FAE}"/>
-    <hyperlink ref="B16" r:id="rId40" xr:uid="{C06489DD-48D7-4AE3-B6B7-E21F87F21567}"/>
-    <hyperlink ref="C16" r:id="rId41" xr:uid="{04FA61CE-8F62-4020-B585-AC6DD3FFD7CD}"/>
-    <hyperlink ref="D16" r:id="rId42" xr:uid="{AA93CF6E-2FF8-4CED-81BA-3A76B37BE3B1}"/>
+    <hyperlink ref="C13" r:id="rId29" xr:uid="{4EE4FA8F-CCC6-4931-8F70-A68DBC9220B2}"/>
+    <hyperlink ref="D13" r:id="rId30" xr:uid="{6176E101-2C7E-46F6-95A3-214967BDD8FE}"/>
+    <hyperlink ref="B14" r:id="rId31" xr:uid="{19E22425-95DB-4A99-A146-142C6BB4A91F}"/>
+    <hyperlink ref="C14" r:id="rId32" xr:uid="{1945C55F-3565-4095-BBC6-E7118079DDDE}"/>
+    <hyperlink ref="D14" r:id="rId33" xr:uid="{944F9636-C8ED-494B-97FF-2206DEA80AB1}"/>
+    <hyperlink ref="B15" r:id="rId34" xr:uid="{7CB51F97-60BB-446D-B2C6-FDDC0C3DC608}"/>
+    <hyperlink ref="C15" r:id="rId35" xr:uid="{1DB6A66C-DE77-4F09-8FE4-E1270AFC0198}"/>
+    <hyperlink ref="D15" r:id="rId36" xr:uid="{3C9CCDBA-C882-4755-B652-2B9EA3B71DDB}"/>
+    <hyperlink ref="B16" r:id="rId37" xr:uid="{C06489DD-48D7-4AE3-B6B7-E21F87F21567}"/>
+    <hyperlink ref="C16" r:id="rId38" xr:uid="{04FA61CE-8F62-4020-B585-AC6DD3FFD7CD}"/>
+    <hyperlink ref="D16" r:id="rId39" xr:uid="{AA93CF6E-2FF8-4CED-81BA-3A76B37BE3B1}"/>
+    <hyperlink ref="B5" r:id="rId40" xr:uid="{02AF2832-AABD-4C24-A0DA-415F92627A77}"/>
+    <hyperlink ref="B13" r:id="rId41" xr:uid="{D5542236-7B7E-483F-B2F8-745442327535}"/>
+    <hyperlink ref="B3" r:id="rId42" xr:uid="{AD83F40E-A405-4B5B-A07E-EB9370D04EDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>